<commit_message>
Modified some data in osama excel sheet
</commit_message>
<xml_diff>
--- a/osama.xlsx
+++ b/osama.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My_Git\Github_Course\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2F7AF0-8C9B-419F-8CAD-59B048EEDEEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,13 +24,28 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>I love Programming and git</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="48"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -49,8 +70,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +354,386 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="D3:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D3:O28"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>